<commit_message>
debug irregular date string
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmware-host\Shared Folders\Documents\pdd-rel\gzt-payroll-pad-vba-v2\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02B0F74-5CDD-4C8D-B143-FE1C9E4330AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71EF93EE-29AA-4D20-8DD9-8C21A46D9516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="1695" windowWidth="21600" windowHeight="12735" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PayrollSchedule" sheetId="1" r:id="rId1"/>
@@ -440,15 +440,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.5" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.625" customWidth="1"/>
     <col min="5" max="5" width="16.125" customWidth="1"/>
     <col min="6" max="6" width="19.25" customWidth="1"/>
@@ -516,13 +516,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>202503</v>
+        <v>202512</v>
       </c>
       <c r="B4" s="1">
-        <v>45741</v>
+        <v>45996</v>
       </c>
       <c r="C4" s="1">
-        <v>45747</v>
+        <v>46020</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -594,7 +594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC3C1246-F39F-43FC-BCFF-FE20EF9521A9}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
codex 5.2增加ui form, pad flow
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -1,33 +1,201 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmware-host\Shared Folders\Documents\pdd-rel\gzt-payroll-pad-vba-v2\config\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71EF93EE-29AA-4D20-8DD9-8C21A46D9516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="17480"/>
   </bookViews>
   <sheets>
-    <sheet name="PayrollSchedule" sheetId="1" r:id="rId1"/>
-    <sheet name="Calendar" sheetId="2" r:id="rId2"/>
-    <sheet name="ExchangeRates" sheetId="3" r:id="rId3"/>
+    <sheet name="Input Files" sheetId="4" r:id="rId1"/>
+    <sheet name="PayrollSchedule" sheetId="1" r:id="rId2"/>
+    <sheet name="Calendar" sheetId="2" r:id="rId3"/>
+    <sheet name="ExchangeRates" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="68">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Keyword</t>
+  </si>
+  <si>
+    <t>FilePath</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>ADP flexiform template_HK_Attendance</t>
+  </si>
+  <si>
+    <t>Attendance</t>
+  </si>
+  <si>
+    <t>process</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>ADP flexiform template_HK_Comp</t>
+  </si>
+  <si>
+    <t>Comp</t>
+  </si>
+  <si>
+    <t>ADP flexiform template_HK_DataChange</t>
+  </si>
+  <si>
+    <t>DataChange</t>
+  </si>
+  <si>
+    <t>ADP flexiform template_HK_NewHire</t>
+  </si>
+  <si>
+    <t>NewHire</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>ADP flexiform template_HK_Termination</t>
+  </si>
+  <si>
+    <t>Termination</t>
+  </si>
+  <si>
+    <t>ADP flexiform template_HK_Variable</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>QX Payout Summary</t>
+  </si>
+  <si>
+    <t>QX_Payout_Summary</t>
+  </si>
+  <si>
+    <t>validation</t>
+  </si>
+  <si>
+    <t>Additional Table</t>
+  </si>
+  <si>
+    <t>Additional_table</t>
+  </si>
+  <si>
+    <t>AIP Payouts Payroll Report</t>
+  </si>
+  <si>
+    <t>AIP</t>
+  </si>
+  <si>
+    <t>Allowance Plan Report</t>
+  </si>
+  <si>
+    <t>Allowance</t>
+  </si>
+  <si>
+    <t>Dividend EY Report</t>
+  </si>
+  <si>
+    <t>Dividend_EY</t>
+  </si>
+  <si>
+    <t>EAO Summary Report</t>
+  </si>
+  <si>
+    <t>EAO_Summary</t>
+  </si>
+  <si>
+    <t>Employee Leave Transactions Report</t>
+  </si>
+  <si>
+    <t>Leave_Transactions</t>
+  </si>
+  <si>
+    <t>Inspire Awards Payroll Report</t>
+  </si>
+  <si>
+    <t>Inspire_Awards</t>
+  </si>
+  <si>
+    <t>Merck Payroll Summary Report</t>
+  </si>
+  <si>
+    <t>Merck_Payroll_Summary_Report_xxx</t>
+  </si>
+  <si>
+    <t>MSD HK Flex Claim Summary Report</t>
+  </si>
+  <si>
+    <t>MSD_Flex_Claim</t>
+  </si>
+  <si>
+    <t>One Time Payment Report</t>
+  </si>
+  <si>
+    <t>One_time_payment</t>
+  </si>
+  <si>
+    <t>Optional Medical Plan Enrollment Form</t>
+  </si>
+  <si>
+    <t>Optional_medical</t>
+  </si>
+  <si>
+    <t>Payroll Report</t>
+  </si>
+  <si>
+    <t>Payroll_Report</t>
+  </si>
+  <si>
+    <t>RSU Dividend EY Report</t>
+  </si>
+  <si>
+    <t>RSU_Dividend_EY</t>
+  </si>
+  <si>
+    <t>RSU Dividend Global Report</t>
+  </si>
+  <si>
+    <t>RSU_Dividend_Global</t>
+  </si>
+  <si>
+    <t>SIP QIP</t>
+  </si>
+  <si>
+    <t>SIP_QIP</t>
+  </si>
+  <si>
+    <t>Workforce Detail - Payroll-AP</t>
+  </si>
+  <si>
+    <t>Workforce_Detail_Payroll_AP</t>
+  </si>
   <si>
     <t>PayrollMonth</t>
   </si>
@@ -71,32 +239,368 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -104,26 +608,319 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+      <numFmt numFmtId="14" formatCode="yyyy/m/d"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+      <numFmt numFmtId="14" formatCode="yyyy/m/d"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="yyyy/m/d"/>
+      <numFmt numFmtId="14" formatCode="yyyy/m/d"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -131,45 +928,42 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DF940FFE-E906-49EE-B66D-11202F16CA27}" name="PayrollSchedule" displayName="PayrollSchedule" ref="A1:F4" totalsRowShown="0">
-  <autoFilter ref="A1:F4" xr:uid="{DF940FFE-E906-49EE-B66D-11202F16CA27}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="PayrollSchedule" displayName="PayrollSchedule" ref="A1:F4" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:F4" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{5878C29C-17ED-40AB-97CC-2F8019099369}" name="PayrollMonth"/>
-    <tableColumn id="2" xr3:uid="{F6AC8AF8-A34E-4498-AE95-012F0AB9140E}" name="CutoffDate" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{A227B878-58AF-4C08-BD67-554C3D98FBA7}" name="PayDate" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{B24FA134-15F3-4C19-BE3F-29FC034BC494}" name="IsAIPMonth"/>
-    <tableColumn id="5" xr3:uid="{27BC9A5C-70B5-4238-93BC-C8E274596DDD}" name="IsRSUDivMonth"/>
-    <tableColumn id="6" xr3:uid="{0BAB7EB1-BD6E-4544-AC53-A57B1CC7D544}" name="IsFlexBenefitMonth"/>
+    <tableColumn id="1" name="PayrollMonth"/>
+    <tableColumn id="2" name="CutoffDate" dataDxfId="0"/>
+    <tableColumn id="3" name="PayDate" dataDxfId="1"/>
+    <tableColumn id="4" name="IsAIPMonth"/>
+    <tableColumn id="5" name="IsRSUDivMonth"/>
+    <tableColumn id="6" name="IsFlexBenefitMonth"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DA3EB179-492B-4ABC-AA9E-C5F5FC031C39}" name="Calendar" displayName="Calendar" ref="A1:B3" totalsRowShown="0">
-  <autoFilter ref="A1:B3" xr:uid="{DA3EB179-492B-4ABC-AA9E-C5F5FC031C39}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Calendar" displayName="Calendar" ref="A1:B3" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:B3" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{0296B750-7B45-4E30-AD29-CE259E46B410}" name="Date" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{B16C4D3B-8E7E-408C-A990-465512DE6961}" name="IsHKHoliday"/>
+    <tableColumn id="1" name="Date" dataDxfId="2"/>
+    <tableColumn id="2" name="IsHKHoliday"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9DB61D96-8A0E-460D-A611-7471E30F959D}" name="ExchangeRates" displayName="ExchangeRates" ref="A1:B4" totalsRowShown="0">
-  <autoFilter ref="A1:B4" xr:uid="{9DB61D96-8A0E-460D-A611-7471E30F959D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="ExchangeRates" displayName="ExchangeRates" ref="A1:B4" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:B4" etc:filterBottomFollowUsedRange="0"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{0EB89231-12BA-4560-A1DD-EE2C973032D4}" name="RateName"/>
-    <tableColumn id="2" xr3:uid="{56CC5E22-D832-4BF6-A6FB-E700C5D4D62D}" name="RateValue"/>
+    <tableColumn id="1" name="RateName"/>
+    <tableColumn id="2" name="RateValue"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -218,7 +1012,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -253,7 +1047,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -427,54 +1221,434 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="16.8" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="37.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="33.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="22.3125" customWidth="1"/>
+    <col min="4" max="4" width="14.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="2" customFormat="1" spans="1:5">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" s="2" customFormat="1" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" s="2" customFormat="1" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" s="2" customFormat="1" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" s="2" customFormat="1" spans="1:5">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" s="2" customFormat="1" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" s="2" customFormat="1" spans="1:5">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" s="2" customFormat="1" spans="1:5">
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" s="2" customFormat="1" spans="1:5">
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" s="2" customFormat="1" spans="1:5">
+      <c r="A10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" s="2" customFormat="1" spans="1:5">
+      <c r="A11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" s="2" customFormat="1" spans="1:5">
+      <c r="A12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" s="2" customFormat="1" spans="1:5">
+      <c r="A13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" s="2" customFormat="1" spans="1:5">
+      <c r="A14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" s="2" customFormat="1" spans="1:5">
+      <c r="A15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" s="2" customFormat="1" spans="1:5">
+      <c r="A16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" s="2" customFormat="1" spans="1:5">
+      <c r="A17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" s="2" customFormat="1" spans="1:5">
+      <c r="A18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" s="2" customFormat="1" spans="1:5">
+      <c r="A19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" s="2" customFormat="1" spans="1:5">
+      <c r="A20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" s="2" customFormat="1" spans="1:5">
+      <c r="A21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" s="2" customFormat="1" spans="1:5">
+      <c r="A22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" s="2" customFormat="1" spans="1:5">
+      <c r="A23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" s="2" customFormat="1" spans="1:5">
+      <c r="A24" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="3" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="14.5" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.125" customWidth="1"/>
     <col min="4" max="4" width="12.625" customWidth="1"/>
     <col min="5" max="5" width="16.125" customWidth="1"/>
     <col min="6" max="6" width="19.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>58</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>59</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>202501</v>
       </c>
@@ -494,7 +1668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>202502</v>
       </c>
@@ -514,7 +1688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>202512</v>
       </c>
@@ -535,55 +1709,8 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6946274B-5111-48DB-ADC0-7A58798FB0FD}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>45658</v>
-      </c>
-      <c r="B2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>45686</v>
-      </c>
-      <c r="B3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -591,54 +1718,103 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC3C1246-F39F-43FC-BCFF-FE20EF9521A9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="13.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>45658</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <v>45686</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
+      <selection activeCell="A1" sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="3" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="11.625" customWidth="1"/>
     <col min="2" max="2" width="11.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="B2">
         <v>7.8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="B3">
         <v>7.8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>

<commit_message>
modify frm mannually and export
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmware-host\Shared Folders\Documents\pdd-rel\gzt-payroll-pad-vba-v2\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A913306F-05B2-4502-8EE6-BF574E9A730C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CF18DD-F7E9-4830-82D4-D7E74AD68D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -230,63 +230,83 @@
   </si>
   <si>
     <t>C:\HK_Payroll\input\1263 ADP flexiform template_HK_Attendance.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>C:\HK_Payroll\input\1263 ADP flexiform template_HK_Comp.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>C:\HK_Payroll\input\1263 ADP flexiform template_HK_DataChange.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>C:\HK_Payroll\input\1263 ADP flexiform template_HK_NewHire.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>C:\HK_Payroll\input\1263 ADP flexiform template_HK_Termination.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>C:\HK_Payroll\input\1263 ADP flexiform template_HK_Variable.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>C:\HK_Payroll\input\Additional table.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>C:\HK_Payroll\input\AIP Payouts Payroll Report.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>C:\HK_Payroll\input\2025\Month\202512\Allowance plan report.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>C:\HK_Payroll\input\Dividend EY report.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>C:\HK_Payroll\input\EAO Summary Report_YYYYMM.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>C:\HK_Payroll\input\Employee_Leave_Transactions_Report.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>C:\HK_Payroll\input\Inspire Awards payroll report.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>C:\HK_Payroll\input\Merck Payroll Summary Report——xxx.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>C:\HK_Payroll\input\One time payment report.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>C:\HK_Payroll\input\2025\Month\202512\Optional medical plan enrollment form.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>C:\HK_Payroll\input\AIP Payouts Payroll Report.xlsx; C:\HK_Payroll\input\Inspire Awards payroll report.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>C:\HK_Payroll\input\RSU Dividend global report.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>C:\HK_Payroll\input\SIP QIP.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>C:\HK_Payroll\input\Workforce Detail - Payroll-AP.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -305,12 +325,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -347,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -357,6 +379,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -714,104 +739,104 @@
       </c>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -831,138 +856,138 @@
       </c>
     </row>
     <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -982,36 +1007,36 @@
       </c>
     </row>
     <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1048,53 +1073,53 @@
       </c>
     </row>
     <row r="22" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="5" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>